<commit_message>
Added machine names and breakdowns
</commit_message>
<xml_diff>
--- a/machine_breakdowns.xlsx
+++ b/machine_breakdowns.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Breakdowns" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="29" customWidth="1" min="1" max="1"/>
+    <col width="28.90625" customWidth="1" min="2" max="2"/>
+    <col width="30.453125" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -469,6 +473,142 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>Overheating</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>V3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Blade Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rivers</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Oil Pressure</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Oil Spring Problem</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Blade Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Blade Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Blade Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ITM2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Blade Guide Problem</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>K4</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Blade Tension</t>
         </is>
       </c>
     </row>

</xml_diff>